<commit_message>
replaced nas with 0
</commit_message>
<xml_diff>
--- a/water-watch/waterwatchapp/coronavirus.xlsx
+++ b/water-watch/waterwatchapp/coronavirus.xlsx
@@ -695,7 +695,9 @@
       <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="s"/>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" t="n">
         <v>29.0000001</v>
       </c>
@@ -729,7 +731,9 @@
         <v>168</v>
       </c>
       <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
@@ -769,7 +773,9 @@
       <c r="G5" t="n">
         <v>4</v>
       </c>
-      <c r="H5" t="s"/>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
       <c r="I5" t="n">
         <v>23.1357694</v>
       </c>
@@ -803,8 +809,12 @@
         <v>132</v>
       </c>
       <c r="F6" t="s"/>
-      <c r="G6" t="s"/>
-      <c r="H6" t="s"/>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
       <c r="I6" t="n">
         <v>30.05518</v>
       </c>
@@ -838,8 +848,12 @@
         <v>106</v>
       </c>
       <c r="F7" t="s"/>
-      <c r="G7" t="s"/>
-      <c r="H7" t="s"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
       <c r="I7" t="n">
         <v>32</v>
       </c>
@@ -873,8 +887,12 @@
         <v>100</v>
       </c>
       <c r="F8" t="s"/>
-      <c r="G8" t="s"/>
-      <c r="H8" t="s"/>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
       <c r="I8" t="n">
         <v>27.9995878</v>
       </c>
@@ -908,8 +926,12 @@
         <v>90</v>
       </c>
       <c r="F9" t="s"/>
-      <c r="G9" t="s"/>
-      <c r="H9" t="s"/>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" t="n">
         <v>30.5000001</v>
       </c>
@@ -943,7 +965,9 @@
         <v>87</v>
       </c>
       <c r="F10" t="s"/>
-      <c r="G10" t="s"/>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
@@ -1022,7 +1046,9 @@
       <c r="G12" t="n">
         <v>2</v>
       </c>
-      <c r="H12" t="s"/>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
       <c r="I12" t="n">
         <v>28</v>
       </c>
@@ -1059,7 +1085,9 @@
       <c r="G13" t="n">
         <v>1</v>
       </c>
-      <c r="H13" t="s"/>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
       <c r="I13" t="n">
         <v>33.0000001</v>
       </c>
@@ -1132,8 +1160,12 @@
         <v>59</v>
       </c>
       <c r="F15" t="s"/>
-      <c r="G15" t="s"/>
-      <c r="H15" t="s"/>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
       <c r="I15" t="n">
         <v>26.5450001</v>
       </c>
@@ -1167,8 +1199,12 @@
         <v>51</v>
       </c>
       <c r="F16" t="s"/>
-      <c r="G16" t="s"/>
-      <c r="H16" t="s"/>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
       <c r="I16" t="n">
         <v>24</v>
       </c>
@@ -1202,8 +1238,12 @@
         <v>35</v>
       </c>
       <c r="F17" t="s"/>
-      <c r="G17" t="s"/>
-      <c r="H17" t="s"/>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
       <c r="I17" t="n">
         <v>36</v>
       </c>
@@ -1237,7 +1277,9 @@
         <v>33</v>
       </c>
       <c r="F18" t="s"/>
-      <c r="G18" t="s"/>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
       <c r="H18" t="n">
         <v>1</v>
       </c>
@@ -1274,7 +1316,9 @@
         <v>33</v>
       </c>
       <c r="F19" t="s"/>
-      <c r="G19" t="s"/>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
       <c r="H19" t="n">
         <v>1</v>
       </c>
@@ -1311,7 +1355,9 @@
         <v>30</v>
       </c>
       <c r="F20" t="s"/>
-      <c r="G20" t="s"/>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
@@ -1348,8 +1394,12 @@
         <v>27</v>
       </c>
       <c r="F21" t="s"/>
-      <c r="G21" t="s"/>
-      <c r="H21" t="s"/>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
       <c r="I21" t="n">
         <v>40.99751970000001</v>
       </c>
@@ -1383,8 +1433,12 @@
         <v>26</v>
       </c>
       <c r="F22" t="s"/>
-      <c r="G22" t="s"/>
-      <c r="H22" t="s"/>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
       <c r="I22" t="n">
         <v>25</v>
       </c>
@@ -1418,8 +1472,12 @@
         <v>23</v>
       </c>
       <c r="F23" t="s"/>
-      <c r="G23" t="s"/>
-      <c r="H23" t="s"/>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
       <c r="I23" t="n">
         <v>39.1235635</v>
       </c>
@@ -1453,8 +1511,12 @@
         <v>20</v>
       </c>
       <c r="F24" t="s"/>
-      <c r="G24" t="s"/>
-      <c r="H24" t="s"/>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
       <c r="I24" t="n">
         <v>37</v>
       </c>
@@ -1488,8 +1550,12 @@
         <v>19</v>
       </c>
       <c r="F25" t="s"/>
-      <c r="G25" t="s"/>
-      <c r="H25" t="s"/>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" t="n">
         <v>38.0000001</v>
       </c>
@@ -1523,8 +1589,12 @@
         <v>11</v>
       </c>
       <c r="F26" t="s"/>
-      <c r="G26" t="s"/>
-      <c r="H26" t="s"/>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
       <c r="I26" t="n">
         <v>43.2443242</v>
       </c>
@@ -1558,8 +1628,12 @@
         <v>9</v>
       </c>
       <c r="F27" t="s"/>
-      <c r="G27" t="s"/>
-      <c r="H27" t="s"/>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
       <c r="I27" t="n">
         <v>27</v>
       </c>
@@ -1593,8 +1667,12 @@
         <v>8</v>
       </c>
       <c r="F28" t="s"/>
-      <c r="G28" t="s"/>
-      <c r="H28" t="s"/>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
       <c r="I28" t="n">
         <v>22.2793278</v>
       </c>
@@ -1628,8 +1706,12 @@
         <v>7</v>
       </c>
       <c r="F29" t="s"/>
-      <c r="G29" t="s"/>
-      <c r="H29" t="s"/>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
       <c r="I29" t="n">
         <v>37.0000001</v>
       </c>
@@ -1663,8 +1745,12 @@
         <v>6</v>
       </c>
       <c r="F30" t="s"/>
-      <c r="G30" t="s"/>
-      <c r="H30" t="s"/>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
       <c r="I30" t="n">
         <v>42.9995032</v>
       </c>
@@ -1698,8 +1784,12 @@
         <v>6</v>
       </c>
       <c r="F31" t="s"/>
-      <c r="G31" t="s"/>
-      <c r="H31" t="s"/>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
       <c r="I31" t="n">
         <v>22.17576</v>
       </c>
@@ -1733,8 +1823,12 @@
         <v>6</v>
       </c>
       <c r="F32" t="s"/>
-      <c r="G32" t="s"/>
-      <c r="H32" t="s"/>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
       <c r="I32" t="n">
         <v>35.40709525</v>
       </c>
@@ -1768,8 +1862,12 @@
         <v>5</v>
       </c>
       <c r="F33" t="s"/>
-      <c r="G33" t="s"/>
-      <c r="H33" t="s"/>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
       <c r="I33" t="n">
         <v>23.9739374</v>
       </c>
@@ -1803,8 +1901,12 @@
         <v>5</v>
       </c>
       <c r="F34" t="s"/>
-      <c r="G34" t="s"/>
-      <c r="H34" t="s"/>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
       <c r="I34" t="n">
         <v>41.7574769</v>
       </c>
@@ -1838,8 +1940,12 @@
         <v>1</v>
       </c>
       <c r="F35" t="s"/>
-      <c r="G35" t="s"/>
-      <c r="H35" t="s"/>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
       <c r="I35" t="n">
         <v>38.89489320000001</v>
       </c>
@@ -1873,8 +1979,12 @@
         <v>1</v>
       </c>
       <c r="F36" t="s"/>
-      <c r="G36" t="s"/>
-      <c r="H36" t="s"/>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
       <c r="I36" t="n">
         <v>40.0796606</v>
       </c>
@@ -1908,8 +2018,12 @@
         <v>2</v>
       </c>
       <c r="F37" t="s"/>
-      <c r="G37" t="s"/>
-      <c r="H37" t="s"/>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
       <c r="I37" t="n">
         <v>36.7014631</v>
       </c>
@@ -1943,8 +2057,12 @@
         <v>1</v>
       </c>
       <c r="F38" t="s"/>
-      <c r="G38" t="s"/>
-      <c r="H38" t="s"/>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
       <c r="I38" t="n">
         <v>34.395342</v>
       </c>
@@ -1981,7 +2099,9 @@
       <c r="G39" t="n">
         <v>1</v>
       </c>
-      <c r="H39" t="s"/>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
       <c r="I39" t="n">
         <v>36.5748441</v>
       </c>
@@ -2018,7 +2138,9 @@
       <c r="G40" t="n">
         <v>2</v>
       </c>
-      <c r="H40" t="s"/>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
       <c r="I40" t="n">
         <v>14.8971921</v>
       </c>
@@ -2052,8 +2174,12 @@
         <v>4</v>
       </c>
       <c r="F41" t="s"/>
-      <c r="G41" t="s"/>
-      <c r="H41" t="s"/>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
       <c r="I41" t="n">
         <v>36.5581914</v>
       </c>
@@ -2087,8 +2213,12 @@
         <v>5</v>
       </c>
       <c r="F42" t="s"/>
-      <c r="G42" t="s"/>
-      <c r="H42" t="s"/>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
       <c r="I42" t="n">
         <v>1.357107</v>
       </c>
@@ -2122,8 +2252,12 @@
         <v>2</v>
       </c>
       <c r="F43" t="s"/>
-      <c r="G43" t="s"/>
-      <c r="H43" t="s"/>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
       <c r="I43" t="n">
         <v>13.2904027</v>
       </c>
@@ -2157,8 +2291,12 @@
         <v>3</v>
       </c>
       <c r="F44" t="s"/>
-      <c r="G44" t="s"/>
-      <c r="H44" t="s"/>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
       <c r="I44" t="n">
         <v>46.603354</v>
       </c>
@@ -2192,8 +2330,12 @@
         <v>1</v>
       </c>
       <c r="F45" t="s"/>
-      <c r="G45" t="s"/>
-      <c r="H45" t="s"/>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
       <c r="I45" t="n">
         <v>28.1083929</v>
       </c>
@@ -2227,8 +2369,12 @@
         <v>4</v>
       </c>
       <c r="F46" t="s"/>
-      <c r="G46" t="s"/>
-      <c r="H46" t="s"/>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
       <c r="I46" t="n">
         <v>4.5693754</v>
       </c>
@@ -2262,8 +2408,12 @@
         <v>1</v>
       </c>
       <c r="F47" t="s"/>
-      <c r="G47" t="s"/>
-      <c r="H47" t="s"/>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
       <c r="I47" t="n">
         <v>50.000678</v>
       </c>
@@ -2297,8 +2447,12 @@
         <v>1</v>
       </c>
       <c r="F48" t="s"/>
-      <c r="G48" t="s"/>
-      <c r="H48" t="s"/>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
       <c r="I48" t="n">
         <v>13.5066394</v>
       </c>
@@ -2332,8 +2486,12 @@
         <v>1</v>
       </c>
       <c r="F49" t="s"/>
-      <c r="G49" t="s"/>
-      <c r="H49" t="s"/>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
       <c r="I49" t="n">
         <v>7.555494199999999</v>
       </c>
@@ -2367,8 +2525,12 @@
         <v>1</v>
       </c>
       <c r="F50" t="s"/>
-      <c r="G50" t="s"/>
-      <c r="H50" t="s"/>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
       <c r="I50" t="n">
         <v>7.9897371</v>
       </c>
@@ -2402,8 +2564,12 @@
         <v>4</v>
       </c>
       <c r="F51" t="s"/>
-      <c r="G51" t="s"/>
-      <c r="H51" t="s"/>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
       <c r="I51" t="n">
         <v>-31.8759835</v>
       </c>
@@ -2437,8 +2603,12 @@
         <v>1</v>
       </c>
       <c r="F52" t="s"/>
-      <c r="G52" t="s"/>
-      <c r="H52" t="s"/>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
       <c r="I52" t="n">
         <v>-36.5986096</v>
       </c>
@@ -2472,8 +2642,12 @@
         <v>1</v>
       </c>
       <c r="F53" t="s"/>
-      <c r="G53" t="s"/>
-      <c r="H53" t="s"/>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
       <c r="I53" t="n">
         <v>48.9467562</v>
       </c>

</xml_diff>